<commit_message>
aggiunto clock gating all
</commit_message>
<xml_diff>
--- a/vivado/Report.xlsx
+++ b/vivado/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco D\universita\magistrale\progettazione-low-power\progetti\progetto-3\vivado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78B1163-F915-42D0-801E-D6D34771C48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059EC5EF-9E7B-4F7F-9FC9-D1A2D290D957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E22A889A-A095-46E2-ACAB-88F50E6B19F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Non Optimized Design</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Clock Gating Inputs Design</t>
+  </si>
+  <si>
+    <t>Clock Gating All Design</t>
+  </si>
+  <si>
+    <t>Hybrid Clock Gating All and Registering Design</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B340A5A-10DF-4AC2-8393-6E0EF86818D6}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,8 +570,7 @@
     <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -729,12 +734,88 @@
         <v>1.3933229027315971E-2</v>
       </c>
     </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>1.4888002770021599E-3</v>
+      </c>
+      <c r="C20" s="6">
+        <v>8.0169141292572004E-3</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3.4701528493314999E-3</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7">
+        <f>B20+C20+D20</f>
+        <v>1.297586725559086E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7">
+        <f>B24+C24+D24</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B22:F22"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiunto hybrid clock gating and registering
</commit_message>
<xml_diff>
--- a/vivado/Report.xlsx
+++ b/vivado/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco D\universita\magistrale\progettazione-low-power\progetti\progetto-3\vivado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059EC5EF-9E7B-4F7F-9FC9-D1A2D290D957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0D768E-78B2-4601-A299-CC50D48E005F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E22A889A-A095-46E2-ACAB-88F50E6B19F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Non Optimized Design</t>
   </si>
@@ -81,7 +81,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,18 +90,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -110,17 +104,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -144,13 +127,19 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -162,24 +151,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -198,32 +169,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,264 +530,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B340A5A-10DF-4AC2-8393-6E0EF86818D6}">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="6">
+        <v>1.7108991742134101E-3</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2.5287989992648402E-3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1.5887991758063401E-3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2.03909818083048E-3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1.4888002770021599E-3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2.01009842567146E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C5" s="6">
+        <v>8.2017192617058806E-3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>7.1427957154810403E-3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8.1042144447565096E-3</v>
+      </c>
+      <c r="F5" s="6">
+        <v>8.0843381583690609E-3</v>
+      </c>
+      <c r="G5" s="6">
+        <v>8.0169141292572004E-3</v>
+      </c>
+      <c r="H5" s="6">
+        <v>7.0602511987090102E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
+      <c r="C6" s="6">
+        <v>3.8697000127285702E-3</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2.55344109609723E-3</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3.6880851257592401E-3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>3.8097926881164299E-3</v>
+      </c>
+      <c r="G6" s="6">
+        <v>3.4701528493314999E-3</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.4122339673340299E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
-        <v>1.7108991742134101E-3</v>
-      </c>
-      <c r="C4" s="6">
-        <v>8.2017192617058806E-3</v>
-      </c>
-      <c r="D4" s="6">
-        <v>3.8697000127285702E-3</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7">
-        <f>B4+C4+D4</f>
+      <c r="C7" s="7">
+        <f>C$4+C$5+C$6</f>
         <v>1.378231844864786E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <v>2.5287989992648402E-3</v>
-      </c>
-      <c r="C8" s="6">
-        <v>7.1427957154810403E-3</v>
-      </c>
-      <c r="D8" s="6">
-        <v>2.55344109609723E-3</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7">
-        <f>B8+C8+D8</f>
+      <c r="D7" s="7">
+        <f>D$4+D$5+D$6</f>
         <v>1.222503581084311E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="E7" s="7">
+        <f>E$4+E$5+E$6</f>
+        <v>1.338109874632209E-2</v>
+      </c>
+      <c r="F7" s="7">
+        <f>F$4+F$5+F$6</f>
+        <v>1.3933229027315971E-2</v>
+      </c>
+      <c r="G7" s="7">
+        <f>G$4+G$5+G$6</f>
+        <v>1.297586725559086E-2</v>
+      </c>
+      <c r="H7" s="7">
+        <f>H$4+H$5+H$6</f>
+        <v>1.14825835917145E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
-        <v>1.5887991758063401E-3</v>
-      </c>
-      <c r="C12" s="6">
-        <v>8.1042144447565096E-3</v>
-      </c>
-      <c r="D12" s="6">
-        <v>3.6880851257592401E-3</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7">
-        <f>B12+C12+D12</f>
-        <v>1.338109874632209E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
-        <v>2.03909818083048E-3</v>
-      </c>
-      <c r="C16" s="6">
-        <v>8.0843381583690609E-3</v>
-      </c>
-      <c r="D16" s="6">
-        <v>3.8097926881164299E-3</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7">
-        <f>B16+C16+D16</f>
-        <v>1.3933229027315971E-2</v>
-      </c>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
-        <v>1.4888002770021599E-3</v>
-      </c>
-      <c r="C20" s="6">
-        <v>8.0169141292572004E-3</v>
-      </c>
-      <c r="D20" s="6">
-        <v>3.4701528493314999E-3</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7">
-        <f>B20+C20+D20</f>
-        <v>1.297586725559086E-2</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7">
-        <f>B24+C24+D24</f>
-        <v>0</v>
-      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B18:F18"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>